<commit_message>
Add device use profile
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-cs.xlsx
+++ b/build/output/StructureDefinition-pacio-cs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="422">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="423">
   <si>
     <t>Path</t>
   </si>
@@ -777,6 +777,10 @@
   </si>
   <si>
     <t>Observation.value[x]</t>
+  </si>
+  <si>
+    <t>Quantity
+CodeableConcept</t>
   </si>
   <si>
     <t>Actual result</t>
@@ -4272,19 +4276,19 @@
         <v>56</v>
       </c>
       <c r="J24" t="s" s="2">
-        <v>164</v>
+        <v>243</v>
       </c>
       <c r="K24" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="O24" t="s" s="2">
         <v>45</v>
@@ -4342,7 +4346,7 @@
         <v>55</v>
       </c>
       <c r="AH24" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="AI24" t="s" s="2">
         <v>67</v>
@@ -4351,24 +4355,24 @@
         <v>45</v>
       </c>
       <c r="AK24" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="AL24" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO24" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="25" hidden="true">
       <c r="A25" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B25" s="2"/>
       <c r="C25" t="s" s="2">
@@ -4394,16 +4398,16 @@
         <v>164</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="N25" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="O25" t="s" s="2">
         <v>45</v>
@@ -4431,10 +4435,10 @@
         <v>179</v>
       </c>
       <c r="X25" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="Y25" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Z25" t="s" s="2">
         <v>45</v>
@@ -4452,7 +4456,7 @@
         <v>45</v>
       </c>
       <c r="AE25" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AF25" t="s" s="2">
         <v>43</v>
@@ -4461,7 +4465,7 @@
         <v>55</v>
       </c>
       <c r="AH25" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AI25" t="s" s="2">
         <v>67</v>
@@ -4476,7 +4480,7 @@
         <v>98</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>45</v>
@@ -4487,11 +4491,11 @@
     </row>
     <row r="26" hidden="true">
       <c r="A26" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B26" s="2"/>
       <c r="C26" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D26" s="2"/>
       <c r="E26" t="s" s="2">
@@ -4513,16 +4517,16 @@
         <v>164</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O26" t="s" s="2">
         <v>45</v>
@@ -4550,10 +4554,10 @@
         <v>179</v>
       </c>
       <c r="X26" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="Y26" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="Z26" t="s" s="2">
         <v>45</v>
@@ -4571,7 +4575,7 @@
         <v>45</v>
       </c>
       <c r="AE26" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AF26" t="s" s="2">
         <v>43</v>
@@ -4589,24 +4593,24 @@
         <v>45</v>
       </c>
       <c r="AK26" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AL26" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="27" hidden="true">
       <c r="A27" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B27" s="2"/>
       <c r="C27" t="s" s="2">
@@ -4629,19 +4633,19 @@
         <v>45</v>
       </c>
       <c r="J27" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="K27" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="O27" t="s" s="2">
         <v>45</v>
@@ -4690,7 +4694,7 @@
         <v>45</v>
       </c>
       <c r="AE27" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="AF27" t="s" s="2">
         <v>43</v>
@@ -4711,10 +4715,10 @@
         <v>45</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AN27" t="s" s="2">
         <v>45</v>
@@ -4725,7 +4729,7 @@
     </row>
     <row r="28" hidden="true">
       <c r="A28" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B28" s="2"/>
       <c r="C28" t="s" s="2">
@@ -4751,13 +4755,13 @@
         <v>164</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="N28" s="2"/>
       <c r="O28" t="s" s="2">
@@ -4783,13 +4787,13 @@
         <v>45</v>
       </c>
       <c r="W28" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="X28" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="Y28" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="Z28" t="s" s="2">
         <v>45</v>
@@ -4807,7 +4811,7 @@
         <v>45</v>
       </c>
       <c r="AE28" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="AF28" t="s" s="2">
         <v>43</v>
@@ -4825,24 +4829,24 @@
         <v>45</v>
       </c>
       <c r="AK28" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="AL28" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="AM28" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="AN28" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO28" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
     </row>
     <row r="29" hidden="true">
       <c r="A29" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" t="s" s="2">
@@ -4868,16 +4872,16 @@
         <v>164</v>
       </c>
       <c r="K29" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="L29" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="M29" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="N29" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="O29" t="s" s="2">
         <v>45</v>
@@ -4902,13 +4906,13 @@
         <v>45</v>
       </c>
       <c r="W29" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="X29" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="Y29" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="Z29" t="s" s="2">
         <v>45</v>
@@ -4926,7 +4930,7 @@
         <v>45</v>
       </c>
       <c r="AE29" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="AF29" t="s" s="2">
         <v>43</v>
@@ -4947,10 +4951,10 @@
         <v>45</v>
       </c>
       <c r="AL29" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="AM29" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="AN29" t="s" s="2">
         <v>45</v>
@@ -4961,7 +4965,7 @@
     </row>
     <row r="30" hidden="true">
       <c r="A30" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="B30" s="2"/>
       <c r="C30" t="s" s="2">
@@ -4984,16 +4988,16 @@
         <v>45</v>
       </c>
       <c r="J30" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="K30" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="L30" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="M30" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="N30" s="2"/>
       <c r="O30" t="s" s="2">
@@ -5043,7 +5047,7 @@
         <v>45</v>
       </c>
       <c r="AE30" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="AF30" t="s" s="2">
         <v>43</v>
@@ -5061,24 +5065,24 @@
         <v>45</v>
       </c>
       <c r="AK30" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AL30" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AM30" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AN30" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO30" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
     </row>
     <row r="31" hidden="true">
       <c r="A31" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B31" s="2"/>
       <c r="C31" t="s" s="2">
@@ -5101,16 +5105,16 @@
         <v>45</v>
       </c>
       <c r="J31" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="K31" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="N31" s="2"/>
       <c r="O31" t="s" s="2">
@@ -5160,7 +5164,7 @@
         <v>45</v>
       </c>
       <c r="AE31" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="AF31" t="s" s="2">
         <v>43</v>
@@ -5178,24 +5182,24 @@
         <v>45</v>
       </c>
       <c r="AK31" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="AL31" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AM31" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="AN31" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO31" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
     </row>
     <row r="32" hidden="true">
       <c r="A32" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B32" s="2"/>
       <c r="C32" t="s" s="2">
@@ -5218,19 +5222,19 @@
         <v>45</v>
       </c>
       <c r="J32" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="K32" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="N32" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="O32" t="s" s="2">
         <v>45</v>
@@ -5279,7 +5283,7 @@
         <v>45</v>
       </c>
       <c r="AE32" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AF32" t="s" s="2">
         <v>43</v>
@@ -5291,7 +5295,7 @@
         <v>45</v>
       </c>
       <c r="AI32" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AJ32" t="s" s="2">
         <v>45</v>
@@ -5300,10 +5304,10 @@
         <v>45</v>
       </c>
       <c r="AL32" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AM32" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AN32" t="s" s="2">
         <v>45</v>
@@ -5314,7 +5318,7 @@
     </row>
     <row r="33" hidden="true">
       <c r="A33" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="B33" s="2"/>
       <c r="C33" t="s" s="2">
@@ -5340,10 +5344,10 @@
         <v>57</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M33" s="2"/>
       <c r="N33" s="2"/>
@@ -5394,7 +5398,7 @@
         <v>45</v>
       </c>
       <c r="AE33" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AF33" t="s" s="2">
         <v>43</v>
@@ -5418,7 +5422,7 @@
         <v>45</v>
       </c>
       <c r="AM33" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AN33" t="s" s="2">
         <v>45</v>
@@ -5429,7 +5433,7 @@
     </row>
     <row r="34" hidden="true">
       <c r="A34" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="B34" s="2"/>
       <c r="C34" t="s" s="2">
@@ -5455,10 +5459,10 @@
         <v>100</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="M34" t="s" s="2">
         <v>120</v>
@@ -5511,7 +5515,7 @@
         <v>45</v>
       </c>
       <c r="AE34" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AF34" t="s" s="2">
         <v>43</v>
@@ -5535,7 +5539,7 @@
         <v>45</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AN34" t="s" s="2">
         <v>45</v>
@@ -5546,11 +5550,11 @@
     </row>
     <row r="35" hidden="true">
       <c r="A35" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="B35" s="2"/>
       <c r="C35" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D35" s="2"/>
       <c r="E35" t="s" s="2">
@@ -5572,10 +5576,10 @@
         <v>100</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="M35" t="s" s="2">
         <v>120</v>
@@ -5630,7 +5634,7 @@
         <v>45</v>
       </c>
       <c r="AE35" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AF35" t="s" s="2">
         <v>43</v>
@@ -5665,7 +5669,7 @@
     </row>
     <row r="36" hidden="true">
       <c r="A36" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B36" s="2"/>
       <c r="C36" t="s" s="2">
@@ -5688,13 +5692,13 @@
         <v>45</v>
       </c>
       <c r="J36" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="K36" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="L36" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="M36" s="2"/>
       <c r="N36" s="2"/>
@@ -5745,7 +5749,7 @@
         <v>45</v>
       </c>
       <c r="AE36" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AF36" t="s" s="2">
         <v>43</v>
@@ -5754,7 +5758,7 @@
         <v>55</v>
       </c>
       <c r="AH36" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="AI36" t="s" s="2">
         <v>67</v>
@@ -5766,10 +5770,10 @@
         <v>45</v>
       </c>
       <c r="AL36" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="AM36" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="AN36" t="s" s="2">
         <v>45</v>
@@ -5780,7 +5784,7 @@
     </row>
     <row r="37" hidden="true">
       <c r="A37" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" t="s" s="2">
@@ -5803,13 +5807,13 @@
         <v>45</v>
       </c>
       <c r="J37" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="K37" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="L37" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="M37" s="2"/>
       <c r="N37" s="2"/>
@@ -5860,7 +5864,7 @@
         <v>45</v>
       </c>
       <c r="AE37" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AF37" t="s" s="2">
         <v>43</v>
@@ -5869,7 +5873,7 @@
         <v>55</v>
       </c>
       <c r="AH37" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="AI37" t="s" s="2">
         <v>67</v>
@@ -5881,10 +5885,10 @@
         <v>45</v>
       </c>
       <c r="AL37" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="AM37" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="AN37" t="s" s="2">
         <v>45</v>
@@ -5895,7 +5899,7 @@
     </row>
     <row r="38" hidden="true">
       <c r="A38" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" t="s" s="2">
@@ -5921,16 +5925,16 @@
         <v>164</v>
       </c>
       <c r="K38" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="N38" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="O38" t="s" s="2">
         <v>45</v>
@@ -5958,10 +5962,10 @@
         <v>79</v>
       </c>
       <c r="X38" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="Y38" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="Z38" t="s" s="2">
         <v>45</v>
@@ -5979,7 +5983,7 @@
         <v>45</v>
       </c>
       <c r="AE38" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AF38" t="s" s="2">
         <v>43</v>
@@ -5997,13 +6001,13 @@
         <v>45</v>
       </c>
       <c r="AK38" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AL38" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AM38" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AN38" t="s" s="2">
         <v>45</v>
@@ -6014,7 +6018,7 @@
     </row>
     <row r="39" hidden="true">
       <c r="A39" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" t="s" s="2">
@@ -6040,16 +6044,16 @@
         <v>164</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="N39" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="O39" t="s" s="2">
         <v>45</v>
@@ -6074,13 +6078,13 @@
         <v>45</v>
       </c>
       <c r="W39" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="X39" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="Z39" t="s" s="2">
         <v>45</v>
@@ -6098,7 +6102,7 @@
         <v>45</v>
       </c>
       <c r="AE39" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="AF39" t="s" s="2">
         <v>43</v>
@@ -6116,13 +6120,13 @@
         <v>45</v>
       </c>
       <c r="AK39" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AL39" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="AM39" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AN39" t="s" s="2">
         <v>45</v>
@@ -6133,7 +6137,7 @@
     </row>
     <row r="40" hidden="true">
       <c r="A40" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" t="s" s="2">
@@ -6156,17 +6160,17 @@
         <v>45</v>
       </c>
       <c r="J40" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="M40" s="2"/>
       <c r="N40" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="O40" t="s" s="2">
         <v>45</v>
@@ -6215,7 +6219,7 @@
         <v>45</v>
       </c>
       <c r="AE40" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="AF40" t="s" s="2">
         <v>43</v>
@@ -6239,7 +6243,7 @@
         <v>45</v>
       </c>
       <c r="AM40" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="AN40" t="s" s="2">
         <v>45</v>
@@ -6250,7 +6254,7 @@
     </row>
     <row r="41" hidden="true">
       <c r="A41" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" t="s" s="2">
@@ -6276,10 +6280,10 @@
         <v>57</v>
       </c>
       <c r="K41" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
@@ -6330,7 +6334,7 @@
         <v>45</v>
       </c>
       <c r="AE41" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="AF41" t="s" s="2">
         <v>43</v>
@@ -6351,10 +6355,10 @@
         <v>45</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="AN41" t="s" s="2">
         <v>45</v>
@@ -6365,7 +6369,7 @@
     </row>
     <row r="42" hidden="true">
       <c r="A42" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" t="s" s="2">
@@ -6388,16 +6392,16 @@
         <v>56</v>
       </c>
       <c r="J42" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="K42" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" t="s" s="2">
@@ -6447,7 +6451,7 @@
         <v>45</v>
       </c>
       <c r="AE42" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="AF42" t="s" s="2">
         <v>43</v>
@@ -6468,10 +6472,10 @@
         <v>45</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="AM42" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="AN42" t="s" s="2">
         <v>45</v>
@@ -6482,7 +6486,7 @@
     </row>
     <row r="43" hidden="true">
       <c r="A43" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" t="s" s="2">
@@ -6505,16 +6509,16 @@
         <v>56</v>
       </c>
       <c r="J43" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="K43" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" t="s" s="2">
@@ -6564,7 +6568,7 @@
         <v>45</v>
       </c>
       <c r="AE43" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="AF43" t="s" s="2">
         <v>43</v>
@@ -6585,10 +6589,10 @@
         <v>45</v>
       </c>
       <c r="AL43" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="AN43" t="s" s="2">
         <v>45</v>
@@ -6599,7 +6603,7 @@
     </row>
     <row r="44" hidden="true">
       <c r="A44" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" t="s" s="2">
@@ -6622,19 +6626,19 @@
         <v>56</v>
       </c>
       <c r="J44" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
       <c r="O44" t="s" s="2">
         <v>45</v>
@@ -6683,7 +6687,7 @@
         <v>45</v>
       </c>
       <c r="AE44" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="AF44" t="s" s="2">
         <v>43</v>
@@ -6704,10 +6708,10 @@
         <v>45</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="AN44" t="s" s="2">
         <v>45</v>
@@ -6718,7 +6722,7 @@
     </row>
     <row r="45" hidden="true">
       <c r="A45" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" t="s" s="2">
@@ -6744,10 +6748,10 @@
         <v>57</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M45" s="2"/>
       <c r="N45" s="2"/>
@@ -6798,7 +6802,7 @@
         <v>45</v>
       </c>
       <c r="AE45" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="AF45" t="s" s="2">
         <v>43</v>
@@ -6822,7 +6826,7 @@
         <v>45</v>
       </c>
       <c r="AM45" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AN45" t="s" s="2">
         <v>45</v>
@@ -6833,7 +6837,7 @@
     </row>
     <row r="46" hidden="true">
       <c r="A46" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" t="s" s="2">
@@ -6859,10 +6863,10 @@
         <v>100</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="M46" t="s" s="2">
         <v>120</v>
@@ -6915,7 +6919,7 @@
         <v>45</v>
       </c>
       <c r="AE46" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="AF46" t="s" s="2">
         <v>43</v>
@@ -6939,7 +6943,7 @@
         <v>45</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>45</v>
@@ -6950,11 +6954,11 @@
     </row>
     <row r="47" hidden="true">
       <c r="A47" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="D47" s="2"/>
       <c r="E47" t="s" s="2">
@@ -6976,10 +6980,10 @@
         <v>100</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="M47" t="s" s="2">
         <v>120</v>
@@ -7034,7 +7038,7 @@
         <v>45</v>
       </c>
       <c r="AE47" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="AF47" t="s" s="2">
         <v>43</v>
@@ -7069,7 +7073,7 @@
     </row>
     <row r="48" hidden="true">
       <c r="A48" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" t="s" s="2">
@@ -7095,13 +7099,13 @@
         <v>164</v>
       </c>
       <c r="K48" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="L48" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="M48" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="N48" t="s" s="2">
         <v>178</v>
@@ -7129,13 +7133,13 @@
         <v>45</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="X48" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="Y48" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>45</v>
@@ -7153,7 +7157,7 @@
         <v>45</v>
       </c>
       <c r="AE48" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="AF48" t="s" s="2">
         <v>55</v>
@@ -7171,7 +7175,7 @@
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>183</v>
@@ -7188,7 +7192,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7211,19 +7215,19 @@
         <v>56</v>
       </c>
       <c r="J49" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="L49" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="N49" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="O49" t="s" s="2">
         <v>45</v>
@@ -7272,7 +7276,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7290,24 +7294,24 @@
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="AL49" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="AM49" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="AN49" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO49" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7333,16 +7337,16 @@
         <v>164</v>
       </c>
       <c r="K50" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="N50" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="O50" t="s" s="2">
         <v>45</v>
@@ -7370,10 +7374,10 @@
         <v>179</v>
       </c>
       <c r="X50" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="Y50" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="Z50" t="s" s="2">
         <v>45</v>
@@ -7391,7 +7395,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7400,7 +7404,7 @@
         <v>55</v>
       </c>
       <c r="AH50" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="AI50" t="s" s="2">
         <v>67</v>
@@ -7415,7 +7419,7 @@
         <v>98</v>
       </c>
       <c r="AM50" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AN50" t="s" s="2">
         <v>45</v>
@@ -7426,11 +7430,11 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="D51" s="2"/>
       <c r="E51" t="s" s="2">
@@ -7452,16 +7456,16 @@
         <v>164</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="O51" t="s" s="2">
         <v>45</v>
@@ -7489,10 +7493,10 @@
         <v>179</v>
       </c>
       <c r="X51" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="Z51" t="s" s="2">
         <v>45</v>
@@ -7510,7 +7514,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7528,24 +7532,24 @@
         <v>45</v>
       </c>
       <c r="AK51" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>45</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7571,16 +7575,16 @@
         <v>45</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="N52" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="O52" t="s" s="2">
         <v>45</v>
@@ -7629,7 +7633,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>
@@ -7650,10 +7654,10 @@
         <v>45</v>
       </c>
       <c r="AL52" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>45</v>

</xml_diff>

<commit_message>
Add CS PHQ9 two-column example to IG web page
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-cs.xlsx
+++ b/build/output/StructureDefinition-pacio-cs.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1943" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1942" uniqueCount="410">
   <si>
     <t>Path</t>
   </si>
@@ -1259,12 +1259,6 @@
   </si>
   <si>
     <t>*All* code-value and  component.code-component.value pairs need to be taken into account to correctly understand the meaning of the observation.</t>
-  </si>
-  <si>
-    <t>Codes identifying names of simple observations.</t>
-  </si>
-  <si>
-    <t>http://hl7.org/fhir/ValueSet/observation-codes</t>
   </si>
   <si>
     <t>&lt; 363787002 |Observable entity| OR @@ -7098,13 +7092,11 @@
         <v>45</v>
       </c>
       <c r="W48" t="s" s="2">
-        <v>280</v>
-      </c>
-      <c r="X48" t="s" s="2">
-        <v>396</v>
-      </c>
+        <v>178</v>
+      </c>
+      <c r="X48" s="2"/>
       <c r="Y48" t="s" s="2">
-        <v>397</v>
+        <v>179</v>
       </c>
       <c r="Z48" t="s" s="2">
         <v>45</v>
@@ -7140,7 +7132,7 @@
         <v>45</v>
       </c>
       <c r="AK48" t="s" s="2">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="AL48" t="s" s="2">
         <v>182</v>
@@ -7157,7 +7149,7 @@
     </row>
     <row r="49" hidden="true">
       <c r="A49" t="s" s="2">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" t="s" s="2">
@@ -7183,13 +7175,13 @@
         <v>163</v>
       </c>
       <c r="K49" t="s" s="2">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="L49" t="s" s="2">
         <v>241</v>
       </c>
       <c r="M49" t="s" s="2">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="N49" t="s" s="2">
         <v>243</v>
@@ -7241,7 +7233,7 @@
         <v>45</v>
       </c>
       <c r="AE49" t="s" s="2">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="AF49" t="s" s="2">
         <v>43</v>
@@ -7259,7 +7251,7 @@
         <v>45</v>
       </c>
       <c r="AK49" t="s" s="2">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="AL49" t="s" s="2">
         <v>246</v>
@@ -7276,7 +7268,7 @@
     </row>
     <row r="50" hidden="true">
       <c r="A50" t="s" s="2">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" t="s" s="2">
@@ -7302,13 +7294,13 @@
         <v>163</v>
       </c>
       <c r="K50" t="s" s="2">
+        <v>402</v>
+      </c>
+      <c r="L50" t="s" s="2">
+        <v>403</v>
+      </c>
+      <c r="M50" t="s" s="2">
         <v>404</v>
-      </c>
-      <c r="L50" t="s" s="2">
-        <v>405</v>
-      </c>
-      <c r="M50" t="s" s="2">
-        <v>406</v>
       </c>
       <c r="N50" t="s" s="2">
         <v>253</v>
@@ -7360,7 +7352,7 @@
         <v>45</v>
       </c>
       <c r="AE50" t="s" s="2">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="AF50" t="s" s="2">
         <v>43</v>
@@ -7395,7 +7387,7 @@
     </row>
     <row r="51" hidden="true">
       <c r="A51" t="s" s="2">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" t="s" s="2">
@@ -7421,7 +7413,7 @@
         <v>163</v>
       </c>
       <c r="K51" t="s" s="2">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="L51" t="s" s="2">
         <v>260</v>
@@ -7479,7 +7471,7 @@
         <v>45</v>
       </c>
       <c r="AE51" t="s" s="2">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="AF51" t="s" s="2">
         <v>43</v>
@@ -7514,7 +7506,7 @@
     </row>
     <row r="52" hidden="true">
       <c r="A52" t="s" s="2">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" t="s" s="2">
@@ -7540,10 +7532,10 @@
         <v>45</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="M52" t="s" s="2">
         <v>314</v>
@@ -7598,7 +7590,7 @@
         <v>45</v>
       </c>
       <c r="AE52" t="s" s="2">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="AF52" t="s" s="2">
         <v>43</v>

</xml_diff>

<commit_message>
Add changes for Block Vote 4 & 5
</commit_message>
<xml_diff>
--- a/build/output/StructureDefinition-pacio-cs.xlsx
+++ b/build/output/StructureDefinition-pacio-cs.xlsx
@@ -490,7 +490,7 @@
     <t>Observation.status</t>
   </si>
   <si>
-    <t>Should have the value 'final' when the observation is complete.</t>
+    <t>Should have the value 'final' when the observation is complete and there are no further actions needed. Otherwise, another value from the value set may appropriately be used.</t>
   </si>
   <si>
     <t>The status of the result value.</t>
@@ -746,7 +746,7 @@
 </t>
   </si>
   <si>
-    <t>The person who performed the assessment. May also be used to provide the practitioner role and organization.</t>
+    <t>The person who performed the assessment. The preferred way to specify the performer is to use the PractitionerRole resource to provide both the practitioner and organization.</t>
   </si>
   <si>
     <t>Who was responsible for asserting the observed value as "true".</t>
@@ -1474,7 +1474,7 @@
     <col min="8" max="8" width="13.2578125" customWidth="true" bestFit="true"/>
     <col min="9" max="9" width="14.44140625" customWidth="true" bestFit="true"/>
     <col min="10" max="10" width="20.703125" customWidth="true" bestFit="true"/>
-    <col min="11" max="11" width="135.2421875" customWidth="true" bestFit="true"/>
+    <col min="11" max="11" width="164.14453125" customWidth="true" bestFit="true"/>
     <col min="12" max="12" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="13" max="13" width="100.703125" customWidth="true" bestFit="true"/>
     <col min="14" max="14" width="100.703125" customWidth="true" bestFit="true"/>
@@ -6447,7 +6447,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="43" hidden="true">
+    <row r="43">
       <c r="A43" t="s" s="2">
         <v>377</v>
       </c>
@@ -6463,7 +6463,7 @@
         <v>44</v>
       </c>
       <c r="G43" t="s" s="2">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="H43" t="s" s="2">
         <v>45</v>

</xml_diff>